<commit_message>
add home page and images
</commit_message>
<xml_diff>
--- a/MudManagement.Server/Db/数据库-泥质.xlsx
+++ b/MudManagement.Server/Db/数据库-泥质.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\05-重点研发计划长江经济带污泥课题\05-调研、图谱\10-数据库\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AB18658-A040-4EB6-9F37-DB1ABB147289}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{866EAC4D-D1A4-43F5-8186-5713B118D716}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5970" yWindow="900" windowWidth="19125" windowHeight="14040" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="基础属性" sheetId="1" r:id="rId1"/>
@@ -2108,8 +2108,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K201"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+    <sheetView topLeftCell="A77" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C103" sqref="C103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2572,7 +2572,7 @@
         <v>28</v>
       </c>
       <c r="C15" s="4">
-        <v>44390.6</v>
+        <v>44390</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>31</v>
@@ -2603,7 +2603,7 @@
         <v>28</v>
       </c>
       <c r="C16" s="4">
-        <v>44390.6</v>
+        <v>44390</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>22</v>
@@ -2634,7 +2634,7 @@
         <v>28</v>
       </c>
       <c r="C17" s="4">
-        <v>44390.6</v>
+        <v>44390</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>22</v>
@@ -2665,7 +2665,7 @@
         <v>28</v>
       </c>
       <c r="C18" s="4">
-        <v>44390.6</v>
+        <v>44390</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>22</v>
@@ -2696,7 +2696,7 @@
         <v>28</v>
       </c>
       <c r="C19" s="4">
-        <v>44390.6</v>
+        <v>44390</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>22</v>
@@ -2727,7 +2727,7 @@
         <v>28</v>
       </c>
       <c r="C20" s="4">
-        <v>44390.6</v>
+        <v>44390</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>22</v>
@@ -3626,7 +3626,7 @@
         <v>39</v>
       </c>
       <c r="C49" s="4">
-        <v>44390.6</v>
+        <v>44390</v>
       </c>
       <c r="D49" s="3" t="s">
         <v>17</v>
@@ -3657,7 +3657,7 @@
         <v>39</v>
       </c>
       <c r="C50" s="4">
-        <v>44390.6</v>
+        <v>44390</v>
       </c>
       <c r="D50" s="3" t="s">
         <v>13</v>
@@ -3688,7 +3688,7 @@
         <v>39</v>
       </c>
       <c r="C51" s="4">
-        <v>44390.6</v>
+        <v>44390</v>
       </c>
       <c r="D51" s="3" t="s">
         <v>12</v>
@@ -3719,7 +3719,7 @@
         <v>39</v>
       </c>
       <c r="C52" s="4">
-        <v>44390.6</v>
+        <v>44390</v>
       </c>
       <c r="D52" s="3" t="s">
         <v>14</v>
@@ -3750,7 +3750,7 @@
         <v>39</v>
       </c>
       <c r="C53" s="4">
-        <v>44390.6</v>
+        <v>44390</v>
       </c>
       <c r="D53" s="3" t="s">
         <v>18</v>
@@ -4680,7 +4680,7 @@
         <v>44</v>
       </c>
       <c r="C83" s="4">
-        <v>44390.6</v>
+        <v>44390</v>
       </c>
       <c r="D83" s="5" t="s">
         <v>7</v>
@@ -4711,7 +4711,7 @@
         <v>44</v>
       </c>
       <c r="C84" s="4">
-        <v>44390.6</v>
+        <v>44390</v>
       </c>
       <c r="D84" s="5" t="s">
         <v>19</v>
@@ -4742,7 +4742,7 @@
         <v>44</v>
       </c>
       <c r="C85" s="4">
-        <v>44390.6</v>
+        <v>44390</v>
       </c>
       <c r="D85" s="5" t="s">
         <v>20</v>
@@ -4773,7 +4773,7 @@
         <v>44</v>
       </c>
       <c r="C86" s="4">
-        <v>44390.6</v>
+        <v>44390</v>
       </c>
       <c r="D86" s="5" t="s">
         <v>21</v>
@@ -8093,8 +8093,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF3F54ED-44C6-4D50-8924-FF49E35A45AB}">
   <dimension ref="A1:O201"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R94" sqref="R94"/>
+    <sheetView topLeftCell="A190" workbookViewId="0">
+      <selection activeCell="C196" sqref="C196"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8725,7 +8725,7 @@
         <v>28</v>
       </c>
       <c r="C15" s="4">
-        <v>44390.6</v>
+        <v>44390</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>31</v>
@@ -8768,7 +8768,7 @@
         <v>28</v>
       </c>
       <c r="C16" s="4">
-        <v>44390.6</v>
+        <v>44390</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>22</v>
@@ -8811,7 +8811,7 @@
         <v>28</v>
       </c>
       <c r="C17" s="4">
-        <v>44390.6</v>
+        <v>44390</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>22</v>
@@ -8854,7 +8854,7 @@
         <v>28</v>
       </c>
       <c r="C18" s="4">
-        <v>44390.6</v>
+        <v>44390</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>22</v>
@@ -8897,7 +8897,7 @@
         <v>28</v>
       </c>
       <c r="C19" s="4">
-        <v>44390.6</v>
+        <v>44390</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>22</v>
@@ -8940,7 +8940,7 @@
         <v>28</v>
       </c>
       <c r="C20" s="4">
-        <v>44390.6</v>
+        <v>44390</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>22</v>
@@ -10163,7 +10163,7 @@
         <v>39</v>
       </c>
       <c r="C49" s="4">
-        <v>44390.6</v>
+        <v>44390</v>
       </c>
       <c r="D49" s="3" t="s">
         <v>17</v>
@@ -10206,7 +10206,7 @@
         <v>39</v>
       </c>
       <c r="C50" s="4">
-        <v>44390.6</v>
+        <v>44390</v>
       </c>
       <c r="D50" s="3" t="s">
         <v>13</v>
@@ -10249,7 +10249,7 @@
         <v>39</v>
       </c>
       <c r="C51" s="4">
-        <v>44390.6</v>
+        <v>44390</v>
       </c>
       <c r="D51" s="3" t="s">
         <v>12</v>
@@ -10292,7 +10292,7 @@
         <v>39</v>
       </c>
       <c r="C52" s="4">
-        <v>44390.6</v>
+        <v>44390</v>
       </c>
       <c r="D52" s="3" t="s">
         <v>14</v>
@@ -10335,7 +10335,7 @@
         <v>39</v>
       </c>
       <c r="C53" s="4">
-        <v>44390.6</v>
+        <v>44390</v>
       </c>
       <c r="D53" s="3" t="s">
         <v>18</v>
@@ -11477,7 +11477,7 @@
         <v>44</v>
       </c>
       <c r="C83" s="4">
-        <v>44390.6</v>
+        <v>44390</v>
       </c>
       <c r="D83" s="5" t="s">
         <v>7</v>
@@ -11520,7 +11520,7 @@
         <v>44</v>
       </c>
       <c r="C84" s="4">
-        <v>44390.6</v>
+        <v>44390</v>
       </c>
       <c r="D84" s="5" t="s">
         <v>19</v>
@@ -11563,7 +11563,7 @@
         <v>44</v>
       </c>
       <c r="C85" s="4">
-        <v>44390.6</v>
+        <v>44390</v>
       </c>
       <c r="D85" s="5" t="s">
         <v>20</v>
@@ -11606,7 +11606,7 @@
         <v>44</v>
       </c>
       <c r="C86" s="4">
-        <v>44390.6</v>
+        <v>44390</v>
       </c>
       <c r="D86" s="5" t="s">
         <v>21</v>
@@ -16302,9 +16302,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DED40034-F344-4B1C-BE1A-220025451F19}">
   <dimension ref="A1:X211"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A177" workbookViewId="0">
       <pane xSplit="4" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H2" sqref="H2"/>
+      <selection pane="topRight" activeCell="C186" sqref="C186"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17336,7 +17336,7 @@
         <v>28</v>
       </c>
       <c r="C15" s="4">
-        <v>44390.6</v>
+        <v>44390</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>31</v>
@@ -17407,7 +17407,7 @@
         <v>28</v>
       </c>
       <c r="C16" s="4">
-        <v>44390.6</v>
+        <v>44390</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>22</v>
@@ -17478,7 +17478,7 @@
         <v>28</v>
       </c>
       <c r="C17" s="4">
-        <v>44390.6</v>
+        <v>44390</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>22</v>
@@ -17549,7 +17549,7 @@
         <v>28</v>
       </c>
       <c r="C18" s="4">
-        <v>44390.6</v>
+        <v>44390</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>22</v>
@@ -17620,7 +17620,7 @@
         <v>28</v>
       </c>
       <c r="C19" s="4">
-        <v>44390.6</v>
+        <v>44390</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>22</v>
@@ -17691,7 +17691,7 @@
         <v>28</v>
       </c>
       <c r="C20" s="4">
-        <v>44390.6</v>
+        <v>44390</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>22</v>
@@ -20313,7 +20313,7 @@
         <v>39</v>
       </c>
       <c r="C58" s="4">
-        <v>44390.6</v>
+        <v>44390</v>
       </c>
       <c r="D58" s="3" t="s">
         <v>17</v>
@@ -20384,7 +20384,7 @@
         <v>39</v>
       </c>
       <c r="C59" s="4">
-        <v>44390.6</v>
+        <v>44390</v>
       </c>
       <c r="D59" s="3" t="s">
         <v>13</v>
@@ -20455,7 +20455,7 @@
         <v>39</v>
       </c>
       <c r="C60" s="4">
-        <v>44390.6</v>
+        <v>44390</v>
       </c>
       <c r="D60" s="3" t="s">
         <v>12</v>
@@ -20526,7 +20526,7 @@
         <v>39</v>
       </c>
       <c r="C61" s="4">
-        <v>44390.6</v>
+        <v>44390</v>
       </c>
       <c r="D61" s="3" t="s">
         <v>14</v>
@@ -20597,7 +20597,7 @@
         <v>39</v>
       </c>
       <c r="C62" s="4">
-        <v>44390.6</v>
+        <v>44390</v>
       </c>
       <c r="D62" s="3" t="s">
         <v>18</v>
@@ -22398,7 +22398,7 @@
         <v>44</v>
       </c>
       <c r="C92" s="4">
-        <v>44390.6</v>
+        <v>44390</v>
       </c>
       <c r="D92" s="5" t="s">
         <v>7</v>
@@ -22469,7 +22469,7 @@
         <v>44</v>
       </c>
       <c r="C93" s="4">
-        <v>44390.6</v>
+        <v>44390</v>
       </c>
       <c r="D93" s="5" t="s">
         <v>19</v>
@@ -22540,7 +22540,7 @@
         <v>44</v>
       </c>
       <c r="C94" s="4">
-        <v>44390.6</v>
+        <v>44390</v>
       </c>
       <c r="D94" s="5" t="s">
         <v>20</v>
@@ -22611,7 +22611,7 @@
         <v>44</v>
       </c>
       <c r="C95" s="4">
-        <v>44390.6</v>
+        <v>44390</v>
       </c>
       <c r="D95" s="5" t="s">
         <v>21</v>
@@ -28514,10 +28514,10 @@
   <dimension ref="A1:X204"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E179" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H195" sqref="H195"/>
+      <selection pane="bottomRight" activeCell="C195" sqref="C195"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -29216,7 +29216,7 @@
         <v>28</v>
       </c>
       <c r="C15" s="4">
-        <v>44390.6</v>
+        <v>44390</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>31</v>
@@ -29248,7 +29248,7 @@
         <v>28</v>
       </c>
       <c r="C16" s="4">
-        <v>44390.6</v>
+        <v>44390</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>22</v>
@@ -29280,7 +29280,7 @@
         <v>28</v>
       </c>
       <c r="C17" s="4">
-        <v>44390.6</v>
+        <v>44390</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>22</v>
@@ -29312,7 +29312,7 @@
         <v>28</v>
       </c>
       <c r="C18" s="4">
-        <v>44390.6</v>
+        <v>44390</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>22</v>
@@ -29344,7 +29344,7 @@
         <v>28</v>
       </c>
       <c r="C19" s="4">
-        <v>44390.6</v>
+        <v>44390</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>22</v>
@@ -29376,7 +29376,7 @@
         <v>28</v>
       </c>
       <c r="C20" s="4">
-        <v>44390.6</v>
+        <v>44390</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>22</v>
@@ -30906,7 +30906,7 @@
         <v>39</v>
       </c>
       <c r="C58" s="4">
-        <v>44390.6</v>
+        <v>44390</v>
       </c>
       <c r="D58" s="3" t="s">
         <v>17</v>
@@ -30938,7 +30938,7 @@
         <v>39</v>
       </c>
       <c r="C59" s="4">
-        <v>44390.6</v>
+        <v>44390</v>
       </c>
       <c r="D59" s="3" t="s">
         <v>13</v>
@@ -30970,7 +30970,7 @@
         <v>39</v>
       </c>
       <c r="C60" s="4">
-        <v>44390.6</v>
+        <v>44390</v>
       </c>
       <c r="D60" s="3" t="s">
         <v>12</v>
@@ -31002,7 +31002,7 @@
         <v>39</v>
       </c>
       <c r="C61" s="4">
-        <v>44390.6</v>
+        <v>44390</v>
       </c>
       <c r="D61" s="3" t="s">
         <v>14</v>
@@ -31034,7 +31034,7 @@
         <v>39</v>
       </c>
       <c r="C62" s="4">
-        <v>44390.6</v>
+        <v>44390</v>
       </c>
       <c r="D62" s="3" t="s">
         <v>18</v>
@@ -32186,7 +32186,7 @@
         <v>44</v>
       </c>
       <c r="C85" s="4">
-        <v>44390.6</v>
+        <v>44390</v>
       </c>
       <c r="D85" s="5" t="s">
         <v>7</v>
@@ -32218,7 +32218,7 @@
         <v>44</v>
       </c>
       <c r="C86" s="4">
-        <v>44390.6</v>
+        <v>44390</v>
       </c>
       <c r="D86" s="5" t="s">
         <v>19</v>
@@ -32250,7 +32250,7 @@
         <v>44</v>
       </c>
       <c r="C87" s="4">
-        <v>44390.6</v>
+        <v>44390</v>
       </c>
       <c r="D87" s="5" t="s">
         <v>20</v>
@@ -32282,7 +32282,7 @@
         <v>44</v>
       </c>
       <c r="C88" s="4">
-        <v>44390.6</v>
+        <v>44390</v>
       </c>
       <c r="D88" s="5" t="s">
         <v>21</v>
@@ -36666,8 +36666,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1F7EA74-2F17-4470-8603-1A26C27DC5E6}">
   <dimension ref="A1:X201"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView topLeftCell="A172" workbookViewId="0">
+      <selection activeCell="C199" sqref="C199"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -37102,7 +37102,7 @@
         <v>28</v>
       </c>
       <c r="C15" s="4">
-        <v>44390.6</v>
+        <v>44390</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>31</v>
@@ -37126,7 +37126,7 @@
         <v>28</v>
       </c>
       <c r="C16" s="4">
-        <v>44390.6</v>
+        <v>44390</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>22</v>
@@ -37150,7 +37150,7 @@
         <v>28</v>
       </c>
       <c r="C17" s="4">
-        <v>44390.6</v>
+        <v>44390</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>22</v>
@@ -37174,7 +37174,7 @@
         <v>28</v>
       </c>
       <c r="C18" s="4">
-        <v>44390.6</v>
+        <v>44390</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>22</v>
@@ -37198,7 +37198,7 @@
         <v>28</v>
       </c>
       <c r="C19" s="4">
-        <v>44390.6</v>
+        <v>44390</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>22</v>
@@ -37222,7 +37222,7 @@
         <v>28</v>
       </c>
       <c r="C20" s="4">
-        <v>44390.6</v>
+        <v>44390</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>22</v>
@@ -38020,7 +38020,7 @@
         <v>39</v>
       </c>
       <c r="C49" s="4">
-        <v>44390.6</v>
+        <v>44390</v>
       </c>
       <c r="D49" s="3" t="s">
         <v>17</v>
@@ -38044,7 +38044,7 @@
         <v>39</v>
       </c>
       <c r="C50" s="4">
-        <v>44390.6</v>
+        <v>44390</v>
       </c>
       <c r="D50" s="3" t="s">
         <v>13</v>
@@ -38068,7 +38068,7 @@
         <v>39</v>
       </c>
       <c r="C51" s="4">
-        <v>44390.6</v>
+        <v>44390</v>
       </c>
       <c r="D51" s="3" t="s">
         <v>12</v>
@@ -38092,7 +38092,7 @@
         <v>39</v>
       </c>
       <c r="C52" s="4">
-        <v>44390.6</v>
+        <v>44390</v>
       </c>
       <c r="D52" s="3" t="s">
         <v>14</v>
@@ -38116,7 +38116,7 @@
         <v>39</v>
       </c>
       <c r="C53" s="4">
-        <v>44390.6</v>
+        <v>44390</v>
       </c>
       <c r="D53" s="3" t="s">
         <v>18</v>
@@ -38908,7 +38908,7 @@
         <v>44</v>
       </c>
       <c r="C83" s="4">
-        <v>44390.6</v>
+        <v>44390</v>
       </c>
       <c r="D83" s="5" t="s">
         <v>7</v>
@@ -38932,7 +38932,7 @@
         <v>44</v>
       </c>
       <c r="C84" s="4">
-        <v>44390.6</v>
+        <v>44390</v>
       </c>
       <c r="D84" s="5" t="s">
         <v>19</v>
@@ -38956,7 +38956,7 @@
         <v>44</v>
       </c>
       <c r="C85" s="4">
-        <v>44390.6</v>
+        <v>44390</v>
       </c>
       <c r="D85" s="5" t="s">
         <v>20</v>
@@ -38980,7 +38980,7 @@
         <v>44</v>
       </c>
       <c r="C86" s="4">
-        <v>44390.6</v>
+        <v>44390</v>
       </c>
       <c r="D86" s="5" t="s">
         <v>21</v>
@@ -41631,7 +41631,7 @@
   <dimension ref="A1:L202"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+      <selection activeCell="G199" sqref="G199"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -42122,7 +42122,7 @@
         <v>28</v>
       </c>
       <c r="C15" s="4">
-        <v>44390.6</v>
+        <v>44390</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>31</v>
@@ -42155,7 +42155,7 @@
         <v>28</v>
       </c>
       <c r="C16" s="4">
-        <v>44390.6</v>
+        <v>44390</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>22</v>
@@ -42188,7 +42188,7 @@
         <v>28</v>
       </c>
       <c r="C17" s="4">
-        <v>44390.6</v>
+        <v>44390</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>22</v>
@@ -42221,7 +42221,7 @@
         <v>28</v>
       </c>
       <c r="C18" s="4">
-        <v>44390.6</v>
+        <v>44390</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>22</v>
@@ -42254,7 +42254,7 @@
         <v>28</v>
       </c>
       <c r="C19" s="4">
-        <v>44390.6</v>
+        <v>44390</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>22</v>
@@ -42287,7 +42287,7 @@
         <v>28</v>
       </c>
       <c r="C20" s="4">
-        <v>44390.6</v>
+        <v>44390</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>22</v>
@@ -43235,7 +43235,7 @@
         <v>39</v>
       </c>
       <c r="C49" s="4">
-        <v>44390.6</v>
+        <v>44390</v>
       </c>
       <c r="D49" s="3" t="s">
         <v>17</v>
@@ -43268,7 +43268,7 @@
         <v>39</v>
       </c>
       <c r="C50" s="4">
-        <v>44390.6</v>
+        <v>44390</v>
       </c>
       <c r="D50" s="3" t="s">
         <v>13</v>
@@ -43301,7 +43301,7 @@
         <v>39</v>
       </c>
       <c r="C51" s="4">
-        <v>44390.6</v>
+        <v>44390</v>
       </c>
       <c r="D51" s="3" t="s">
         <v>12</v>
@@ -43334,7 +43334,7 @@
         <v>39</v>
       </c>
       <c r="C52" s="4">
-        <v>44390.6</v>
+        <v>44390</v>
       </c>
       <c r="D52" s="3" t="s">
         <v>14</v>
@@ -43367,7 +43367,7 @@
         <v>39</v>
       </c>
       <c r="C53" s="4">
-        <v>44390.6</v>
+        <v>44390</v>
       </c>
       <c r="D53" s="3" t="s">
         <v>18</v>
@@ -44294,7 +44294,7 @@
         <v>44</v>
       </c>
       <c r="C83" s="4">
-        <v>44390.6</v>
+        <v>44390</v>
       </c>
       <c r="D83" s="5" t="s">
         <v>7</v>
@@ -44327,7 +44327,7 @@
         <v>44</v>
       </c>
       <c r="C84" s="4">
-        <v>44390.6</v>
+        <v>44390</v>
       </c>
       <c r="D84" s="5" t="s">
         <v>19</v>
@@ -44360,7 +44360,7 @@
         <v>44</v>
       </c>
       <c r="C85" s="4">
-        <v>44390.6</v>
+        <v>44390</v>
       </c>
       <c r="D85" s="5" t="s">
         <v>20</v>
@@ -44393,7 +44393,7 @@
         <v>44</v>
       </c>
       <c r="C86" s="4">
-        <v>44390.6</v>
+        <v>44390</v>
       </c>
       <c r="D86" s="5" t="s">
         <v>21</v>

</xml_diff>